<commit_message>
file excel test bootstrap
</commit_message>
<xml_diff>
--- a/others/Dev Shapley/index.xlsx
+++ b/others/Dev Shapley/index.xlsx
@@ -7,48 +7,23 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Shapley" sheetId="1" r:id="rId1"/>
-    <sheet name="First_sobol" sheetId="2" r:id="rId2"/>
-    <sheet name="Total_sobol" sheetId="3" r:id="rId3"/>
+    <sheet name="Ni_3_boot_3_index1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ni_3_boot_3_index2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
-    <t>X1</t>
+    <t>Sh</t>
   </si>
   <si>
-    <t>X2</t>
+    <t>ICmin</t>
   </si>
   <si>
-    <t>X3</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>2.5%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
-    <t>97.5%</t>
-  </si>
-  <si>
-    <t>max</t>
+    <t>ICmax</t>
   </si>
 </sst>
 </file>
@@ -406,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -424,115 +399,45 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0.1032088428581094</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>0.01956494163856978</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>0.03806625757929533</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.177733082624527</v>
+        <v>0.4236416899038825</v>
       </c>
       <c r="C3">
-        <v>0.390458175872535</v>
+        <v>0.4395637996740079</v>
       </c>
       <c r="D3">
-        <v>0.431808741502938</v>
+        <v>0.4605008457908788</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0238685706366309</v>
+        <v>0.4731494672380082</v>
       </c>
       <c r="C4">
-        <v>0.0090026478191105</v>
+        <v>0.5138410500791554</v>
       </c>
       <c r="D4">
-        <v>0.0153804045513161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.113737556964063</v>
-      </c>
-      <c r="C5">
-        <v>0.381605232704691</v>
-      </c>
-      <c r="D5">
-        <v>0.41844122080005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.127762880795542</v>
-      </c>
-      <c r="C6">
-        <v>0.381953577724269</v>
-      </c>
-      <c r="D6">
-        <v>0.419047199158951</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.180047457691211</v>
-      </c>
-      <c r="C7">
-        <v>0.388586311566773</v>
-      </c>
-      <c r="D7">
-        <v>0.429069202433923</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.19899922311678</v>
-      </c>
-      <c r="C8">
-        <v>0.409246949276133</v>
-      </c>
-      <c r="D8">
-        <v>0.46416717190722</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.199953546495259</v>
-      </c>
-      <c r="C9">
-        <v>0.412859596829147</v>
-      </c>
-      <c r="D9">
-        <v>0.473402846206791</v>
+        <v>0.5265826883667725</v>
       </c>
     </row>
   </sheetData>
@@ -542,7 +447,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -560,251 +465,45 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0.1032088428581094</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>0.0213376286757459</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>0.03557481390393211</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.387248954506272</v>
+        <v>0.4236416899038825</v>
       </c>
       <c r="C3">
-        <v>0.873002824902709</v>
+        <v>0.4487536080444519</v>
       </c>
       <c r="D3">
-        <v>0.915764754485297</v>
+        <v>0.4586448748009894</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0927398938923771</v>
+        <v>0.4731494672380082</v>
       </c>
       <c r="C4">
-        <v>0.0198148389638818</v>
+        <v>0.511581477632209</v>
       </c>
       <c r="D4">
-        <v>0.0131519484784222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.131824403078311</v>
-      </c>
-      <c r="C5">
-        <v>0.817214471440274</v>
-      </c>
-      <c r="D5">
-        <v>0.87900057285253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.189998015894555</v>
-      </c>
-      <c r="C6">
-        <v>0.830275661848735</v>
-      </c>
-      <c r="D6">
-        <v>0.887457592093652</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.403323934175013</v>
-      </c>
-      <c r="C7">
-        <v>0.877954211631199</v>
-      </c>
-      <c r="D7">
-        <v>0.91969338108194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.454752541371242</v>
-      </c>
-      <c r="C8">
-        <v>0.883882837060006</v>
-      </c>
-      <c r="D8">
-        <v>0.923676626743044</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.455246620489048</v>
-      </c>
-      <c r="C9">
-        <v>0.884205494728792</v>
-      </c>
-      <c r="D9">
-        <v>0.924285178419942</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.0733705489601034</v>
-      </c>
-      <c r="C3">
-        <v>0.0136584175609126</v>
-      </c>
-      <c r="D3">
-        <v>0.0558247445167527</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.0113915880302005</v>
-      </c>
-      <c r="C4">
-        <v>0.00220090573127392</v>
-      </c>
-      <c r="D4">
-        <v>0.00858622929458632</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.0660650795983828</v>
-      </c>
-      <c r="C5">
-        <v>0.0122932416395923</v>
-      </c>
-      <c r="D5">
-        <v>0.0509605934478707</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>0.0663159648605461</v>
-      </c>
-      <c r="C6">
-        <v>0.0123544624363958</v>
-      </c>
-      <c r="D6">
-        <v>0.0511157833065558</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0.069440614229883</v>
-      </c>
-      <c r="C7">
-        <v>0.0130591779899146</v>
-      </c>
-      <c r="D7">
-        <v>0.0532066291070618</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>0.0980383069747309</v>
-      </c>
-      <c r="C8">
-        <v>0.01842385544951</v>
-      </c>
-      <c r="D8">
-        <v>0.0744529359339849</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0.104714879357229</v>
-      </c>
-      <c r="C9">
-        <v>0.0198179049253647</v>
-      </c>
-      <c r="D9">
-        <v>0.0799321938901308</v>
+        <v>0.5231168276303948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>